<commit_message>
a bit of buffer research
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA44F52-3450-4A5F-B450-C0EB7936D5DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58E3D6-FB67-40D8-8215-C2C82638DCA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Projekt Redpitaya Oszilloskop</t>
   </si>
   <si>
-    <t>Dienstag 27.10.2020</t>
-  </si>
-  <si>
     <t>Absprache mit Prof. Münch bzgl. Themenfindung</t>
   </si>
   <si>
@@ -67,38 +64,26 @@
 Redpitaya, Connection RP und VM</t>
   </si>
   <si>
-    <t>Donnerstag 29.10.2020</t>
-  </si>
-  <si>
-    <t>Donnerstag 05.11.2020</t>
-  </si>
-  <si>
     <t>Introduction zur Programmierung, Pinout, 
 HF In-Output Ansteuerung</t>
   </si>
   <si>
-    <t>Dienstag 10.11.2020</t>
-  </si>
-  <si>
     <t>Zoom Meeting Prof. Münch (Zwischenstand)</t>
   </si>
   <si>
-    <t>Donnerstag 12.11.2020</t>
-  </si>
-  <si>
     <t>Interne Absprache, Arbeitsaufteilung</t>
   </si>
   <si>
-    <t>Dienstag 17.11.2020</t>
-  </si>
-  <si>
     <t>Vorbereitung Stresstest und Input-Auslesen verstehen</t>
   </si>
   <si>
-    <t>Donnerstag 19.11.2020</t>
-  </si>
-  <si>
-    <t>Stresstest durchgeführt (Auslesen klappt ohne Probleme). Tieferes einlesen in rp.h library (Abtastraten , …)</t>
+    <t>Stresstest durchgeführt. Tieferes einlesen in rp.h library (Abtastraten , Buffer, …)</t>
+  </si>
+  <si>
+    <t>Zoom Meeting</t>
+  </si>
+  <si>
+    <t>recherchen buffer(auslesen und schreiben, ..), rp.h</t>
   </si>
 </sst>
 </file>
@@ -151,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -165,6 +150,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,37 +471,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -542,8 +528,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
+      <c r="A5" s="5">
+        <v>44131</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -553,12 +539,12 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
+      <c r="A6" s="5">
+        <v>44133</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -568,12 +554,12 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
+      <c r="A7" s="5">
+        <v>44140</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -583,12 +569,12 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
+      <c r="A8" s="5">
+        <v>44145</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -598,12 +584,12 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="A9" s="5">
+        <v>44147</v>
       </c>
       <c r="B9">
         <v>2.5</v>
@@ -613,12 +599,12 @@
         <v>13.5</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
+      <c r="A10" s="5">
+        <v>44152</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -628,22 +614,52 @@
         <v>15.5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>44154</v>
       </c>
       <c r="B11">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <f>B11+C10</f>
-        <v>18</v>
+        <v>18.5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>44159</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>B12+C11</f>
+        <v>19.5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>44160</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>B13+C12</f>
+        <v>21.5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redpitaya update + homeoffice integration
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\OTH\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A57AF2-D4D5-444D-91AD-3946EBA6F9F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D95E5D-2891-4B11-90F5-EE42EF186AA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="6615" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>versucht signal in webapp zu lesen und zu senden</t>
+  </si>
+  <si>
+    <t>zweiwöchentliches Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redpitaya abgeholt, upgedated und in HomeOffice Arbeitsplatz integriert </t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <f>B10+C9</f>
+        <f t="shared" ref="C10:C16" si="1">B10+C9</f>
         <v>15.5</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -631,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <f>B11+C10</f>
+        <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -646,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <f>B12+C11</f>
+        <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -661,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <f>B13+C12</f>
+        <f t="shared" si="1"/>
         <v>21.5</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -676,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="C14">
-        <f>B14+C13</f>
+        <f t="shared" si="1"/>
         <v>25.5</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -691,11 +697,41 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <f>B15+C14</f>
+        <f t="shared" si="1"/>
         <v>28.5</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>44173</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>44182</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <f>C16+B17</f>
+        <v>33.5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated stundenliste + saved signalgeneration example
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D95E5D-2891-4B11-90F5-EE42EF186AA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD5152-91C0-419D-8DAA-AC4FFD89619F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="360" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -96,6 +96,10 @@
   </si>
   <si>
     <t xml:space="preserve">redpitaya abgeholt, upgedated und in HomeOffice Arbeitsplatz integriert </t>
+  </si>
+  <si>
+    <t>Interne Absprache, Planung weiteres vorghen
+Quellcodes auf neuen Redpitaya geschrieben und Funktion getestet</t>
   </si>
 </sst>
 </file>
@@ -483,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,14 +728,29 @@
         <v>44182</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <f>C16+B17</f>
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>44183</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f>B18+C17</f>
+        <v>36.5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried vpn but failed, so updated hours only
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63592005-41E9-43E3-AAB7-1ECED92285F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D888FB7E-33F0-45F0-AD29-0A74EAC1C8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -100,6 +100,9 @@
   <si>
     <t>Interne Absprache, Planung weiteres vorghen
 Quellcodes auf neuen Redpitaya geschrieben und Datenaquirierung debugged</t>
+  </si>
+  <si>
+    <t>Versucht Redpitaya per VPN, über Florians wireguard verfügbar zu machen. --&gt; keine kernel headers für 4.9.0-xilinx und kein module support..</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,6 +756,21 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>44185</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <f>C18+B19</f>
+        <v>41.5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
vpn mit Raspberry und versuchtem bridgen
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830D7F6E-60EE-4FEA-9636-71638F41D612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A3DBB6-90AB-4E63-AFD0-B6593B45AF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -103,6 +103,13 @@
   </si>
   <si>
     <t>Versucht Redpitaya per VPN, über Florians wireguard verfügbar zu machen. --&gt; keine kernel headers für 4.9.0-xilinx und kein module support..</t>
+  </si>
+  <si>
+    <t>Raspberry für VPN eingerichtet und über wireguard verbunden</t>
+  </si>
+  <si>
+    <t>Versucht VPN verbindung auf Redpitaya weiterzugeben
+Entweder fehler beim bridgen oder Redpitaya bekam immer eigene IP-Adresse ohne VPN</t>
   </si>
 </sst>
 </file>
@@ -490,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,6 +793,36 @@
         <v>18</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>44194</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f>C20+B21</f>
+        <v>45.5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f>C21+B22</f>
+        <v>49.5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
windows fails gefixt, luguru, ...
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29449341-E1C7-439B-B222-F5D769CB1497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C54F0-1CEC-485A-BE30-718EFAE9A1B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Datum</t>
   </si>
@@ -123,6 +123,10 @@
   </si>
   <si>
     <t>Initiale Dokumentation erstellt &amp; Klassendiagramm reviewed</t>
+  </si>
+  <si>
+    <t>Klassendiagramm besprochen, StateChart, Arbeitsaufteilung, loguru in App integriert.
+NEVER USE WINDOWS (daraus resultierte Fehler gefixt)</t>
   </si>
 </sst>
 </file>
@@ -510,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:C27" si="2">C18+B19</f>
+        <f t="shared" ref="C19:C28" si="2">C18+B19</f>
         <v>41.5</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -909,6 +913,21 @@
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>44224</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>80.5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added interface, add headers in cmake
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24331"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C91BAC-3769-4613-8FDC-D605F400E126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{C9866062-247D-428B-806A-F231CEA3B0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20598741-52C3-44AC-A483-C4A17286CEDF}"/>
   <bookViews>
     <workbookView xWindow="32400" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Studenliste von Michael Schneider</t>
   </si>
@@ -101,26 +101,39 @@
     <t>bug fixing, parsing empfangene optionen, testing</t>
   </si>
   <si>
+    <t>Meeting + testing</t>
+  </si>
+  <si>
+    <t>internes Meeting + codeanalyse</t>
+  </si>
+  <si>
+    <t>fixed strange npm error (dokumentiert aber unklar, was und wieso)</t>
+  </si>
+  <si>
+    <t>empfangen und parsen fertig gestellt, minor bugs gefixt</t>
+  </si>
+  <si>
+    <t>Parameteranpassung, Decimation aus sampleRate generieren
+Bug versucht nachzustellen, erfolglos</t>
+  </si>
+  <si>
+    <t>internes Meeting + Meeting mit Prof. Münch</t>
+  </si>
+  <si>
+    <t>reguläres internes Meeting</t>
+  </si>
+  <si>
+    <t>zusatzmeeting (erhöhter Bedarf nach Prüfungsphasenpause)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Meeting + testing</t>
-  </si>
-  <si>
-    <t>internes Meeting + codeanalyse</t>
-  </si>
-  <si>
-    <t>fixed strange npm error (dokumentiert aber unklar, was und wieso)</t>
-  </si>
-  <si>
-    <t>empfangen und parsen fertig gestellt, minor bugs gefixt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +158,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,20 +193,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -197,15 +211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -224,7 +236,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,47 +535,47 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -576,26 +588,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:5" ht="30">
+      <c r="A5" s="6">
         <v>44273</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>44274</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>7</v>
       </c>
       <c r="C6">
@@ -606,11 +618,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>44287</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>3</v>
       </c>
       <c r="C7">
@@ -621,11 +633,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>44292</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>2</v>
       </c>
       <c r="C8">
@@ -636,11 +648,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>44294</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>4</v>
       </c>
       <c r="C9">
@@ -651,11 +663,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>44301</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>6</v>
       </c>
       <c r="C10">
@@ -666,26 +678,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>44308</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11">
         <v>3</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C22" si="0">C10+B11</f>
+        <f t="shared" ref="C11:C26" si="0">C10+B11</f>
         <v>28</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>44315</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12">
         <v>4</v>
       </c>
       <c r="C12">
@@ -696,11 +708,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>44318</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13">
         <v>3</v>
       </c>
       <c r="C13">
@@ -711,11 +723,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>44328</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14">
         <v>4</v>
       </c>
       <c r="C14">
@@ -726,11 +738,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>44336</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15">
         <v>3</v>
       </c>
       <c r="C15">
@@ -741,11 +753,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>44337</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
@@ -756,11 +768,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="3">
         <v>44342</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
@@ -771,11 +783,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="3">
         <v>44350</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18">
         <v>5</v>
       </c>
       <c r="C18">
@@ -786,11 +798,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="3">
         <v>44357</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19">
         <v>2</v>
       </c>
       <c r="C19">
@@ -798,14 +810,14 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="3">
         <v>44364</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20">
         <v>2</v>
       </c>
       <c r="C20">
@@ -813,14 +825,14 @@
         <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="3">
         <v>44373</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21">
         <v>3</v>
       </c>
       <c r="C21">
@@ -828,14 +840,14 @@
         <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="3">
         <v>44374</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22">
         <v>5</v>
       </c>
       <c r="C22">
@@ -843,87 +855,134 @@
         <v>63</v>
       </c>
       <c r="D22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30">
+      <c r="A23" s="3">
+        <v>44377</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
+      <c r="A24" s="3">
+        <v>44378</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3">
+        <v>44406</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3">
+        <v>44412</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="3"/>
-      <c r="B30"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="3"/>
       <c r="E33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not sure what these changes are
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-MichaelSchneider.xlsx
+++ b/stundenlisten/Stundenliste-MichaelSchneider.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/477ec295378db8c3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\OTH\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{92742F7E-4624-4D3B-838C-365B285E10C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B7316FC-087F-4F21-AB6E-BB9DF1D5866A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2D8E7-1433-45E0-B7F3-5CB2CE654BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Projekt Redpitaya Oszilloskop</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Stundenliste von Michael Schneider</t>
+  </si>
+  <si>
+    <t>internes meeting</t>
+  </si>
+  <si>
+    <t>Dokumentation, tests</t>
+  </si>
+  <si>
+    <t>Klassendiagramm gecheckt und updated</t>
   </si>
 </sst>
 </file>
@@ -576,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +737,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C39" si="0">C10+B11</f>
+        <f t="shared" ref="C11:C42" si="0">C10+B11</f>
         <v>28</v>
       </c>
       <c r="D11" t="s">
@@ -1159,13 +1168,49 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="3">
+        <v>44445</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="3">
+        <v>44446</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="3">
+        <v>44448</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>

</xml_diff>